<commit_message>
fix stepcount on Turndup (SX 13)
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67DF48F8-EDD3-44DB-8C0B-2787232ECA94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F85DFE-0382-4884-A29C-52688A0148D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -3399,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
   <dimension ref="A1:E607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E473" sqref="E473:E478"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B473" sqref="B473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9803,7 +9803,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="377" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A377" s="6" t="s">
         <v>381</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>476</v>
       </c>
       <c r="B472" s="12">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C472" s="12">
         <v>13</v>

</xml_diff>

<commit_message>
songlist update april 3, 2021
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6858B4E5-3444-4C1A-B913-1FDC63EB42B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2763E148-CA06-49F4-A971-177705076606}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="1074">
   <si>
     <t>Rapid Fire (SH 7)</t>
   </si>
@@ -3124,6 +3124,138 @@
   </si>
   <si>
     <t>Vintage Circuit (SX 14)</t>
+  </si>
+  <si>
+    <t>Disconnected Disco (SH)</t>
+  </si>
+  <si>
+    <t>Da Roots (folk mix)</t>
+  </si>
+  <si>
+    <t>Ride the Bass</t>
+  </si>
+  <si>
+    <t>Rom-eo &amp; Juli8</t>
+  </si>
+  <si>
+    <t>Wake Up</t>
+  </si>
+  <si>
+    <t>Vi Sitter I Ventrilo Och Spelar DotA</t>
+  </si>
+  <si>
+    <t>Oasis</t>
+  </si>
+  <si>
+    <t>Soapy Bubble</t>
+  </si>
+  <si>
+    <t>Stop the Music</t>
+  </si>
+  <si>
+    <t>Sweet World</t>
+  </si>
+  <si>
+    <t>Twilight</t>
+  </si>
+  <si>
+    <t>Disconnected Sanxion7 remix</t>
+  </si>
+  <si>
+    <t>Monolith</t>
+  </si>
+  <si>
+    <t>Robotix</t>
+  </si>
+  <si>
+    <t>The Man Crossing The Channel</t>
+  </si>
+  <si>
+    <t>Determinator</t>
+  </si>
+  <si>
+    <t>Euphoria</t>
+  </si>
+  <si>
+    <t>Over The Rave</t>
+  </si>
+  <si>
+    <t>We Met Dat Night</t>
+  </si>
+  <si>
+    <t>Epileptic Crisis</t>
+  </si>
+  <si>
+    <t>Pandemonium</t>
+  </si>
+  <si>
+    <t>Chromatic Blitz</t>
+  </si>
+  <si>
+    <t>Disconnected Disco (SH 8)</t>
+  </si>
+  <si>
+    <t>Da Roots (SX 9)</t>
+  </si>
+  <si>
+    <t>Ride the Bass (SX 9)</t>
+  </si>
+  <si>
+    <t>ROM-eo _ Juli8 (SX 9)</t>
+  </si>
+  <si>
+    <t>Vi Sitter I Ventrilo Och Spelar DotA (SX 9)</t>
+  </si>
+  <si>
+    <t>Wake Up (SX 9)</t>
+  </si>
+  <si>
+    <t>Oasis (SX 10)</t>
+  </si>
+  <si>
+    <t>Soapy Bubble (SX 10)</t>
+  </si>
+  <si>
+    <t>Stop the Music (SX 10)</t>
+  </si>
+  <si>
+    <t>Sweet World (SX 10)</t>
+  </si>
+  <si>
+    <t>Twilight (SX 10)</t>
+  </si>
+  <si>
+    <t>Disconnected (Sanxion7 remix) (SX 11)</t>
+  </si>
+  <si>
+    <t>Monolith (SX 11)</t>
+  </si>
+  <si>
+    <t>Robotix (SX 11)</t>
+  </si>
+  <si>
+    <t>The Man Crossing the Channel (SX 11)</t>
+  </si>
+  <si>
+    <t>We Met Dat Night (SX 12)</t>
+  </si>
+  <si>
+    <t>Epileptic Crisis (SX 13)</t>
+  </si>
+  <si>
+    <t>Pandemonium (SX 13)</t>
+  </si>
+  <si>
+    <t>Chromatic Blitz (SX 14)</t>
+  </si>
+  <si>
+    <t>Determinator (SX 12)</t>
+  </si>
+  <si>
+    <t>Euphoria (SX 12)</t>
+  </si>
+  <si>
+    <t>Over the Rave (SX 12)</t>
   </si>
 </sst>
 </file>
@@ -3180,7 +3312,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3202,6 +3334,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4FFE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3293,7 +3431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3351,6 +3489,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3674,8 +3821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
   <dimension ref="A1:E607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A502" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E512" sqref="E512"/>
+    <sheetView tabSelected="1" topLeftCell="A520" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E533" sqref="E533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12425,202 +12572,378 @@
       </c>
     </row>
     <row r="515" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A515" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B515" s="9"/>
-      <c r="C515" s="9"/>
-      <c r="D515" s="9"/>
-      <c r="E515" s="2"/>
+      <c r="A515" s="21" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B515" s="22">
+        <v>391</v>
+      </c>
+      <c r="C515" s="22">
+        <v>0</v>
+      </c>
+      <c r="D515" s="22">
+        <v>5</v>
+      </c>
+      <c r="E515" s="23" t="s">
+        <v>1052</v>
+      </c>
     </row>
     <row r="516" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A516" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B516" s="9"/>
-      <c r="C516" s="9"/>
-      <c r="D516" s="9"/>
-      <c r="E516" s="2"/>
+      <c r="A516" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B516" s="22">
+        <v>489</v>
+      </c>
+      <c r="C516" s="22">
+        <v>0</v>
+      </c>
+      <c r="D516" s="22">
+        <v>4</v>
+      </c>
+      <c r="E516" s="23" t="s">
+        <v>1053</v>
+      </c>
     </row>
     <row r="517" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A517" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B517" s="9"/>
-      <c r="C517" s="9"/>
-      <c r="D517" s="9"/>
-      <c r="E517" s="2"/>
+      <c r="A517" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B517" s="22">
+        <v>385</v>
+      </c>
+      <c r="C517" s="22">
+        <v>0</v>
+      </c>
+      <c r="D517" s="22">
+        <v>26</v>
+      </c>
+      <c r="E517" s="23" t="s">
+        <v>1054</v>
+      </c>
     </row>
     <row r="518" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A518" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B518" s="9"/>
-      <c r="C518" s="9"/>
-      <c r="D518" s="9"/>
-      <c r="E518" s="2"/>
+      <c r="A518" s="21" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B518" s="22">
+        <v>459</v>
+      </c>
+      <c r="C518" s="22">
+        <v>0</v>
+      </c>
+      <c r="D518" s="22">
+        <v>41</v>
+      </c>
+      <c r="E518" s="23" t="s">
+        <v>1055</v>
+      </c>
     </row>
     <row r="519" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A519" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B519" s="9"/>
-      <c r="C519" s="9"/>
-      <c r="D519" s="9"/>
-      <c r="E519" s="2"/>
-    </row>
-    <row r="520" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A520" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B520" s="9"/>
-      <c r="C520" s="9"/>
-      <c r="D520" s="9"/>
-      <c r="E520" s="2"/>
+      <c r="A519" s="21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B519" s="22">
+        <v>426</v>
+      </c>
+      <c r="C519" s="22">
+        <v>0</v>
+      </c>
+      <c r="D519" s="22">
+        <v>40</v>
+      </c>
+      <c r="E519" s="23" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A520" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B520" s="22">
+        <v>391</v>
+      </c>
+      <c r="C520" s="22">
+        <v>4</v>
+      </c>
+      <c r="D520" s="22">
+        <v>4</v>
+      </c>
+      <c r="E520" s="23" t="s">
+        <v>1056</v>
+      </c>
     </row>
     <row r="521" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A521" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B521" s="9"/>
-      <c r="C521" s="9"/>
-      <c r="D521" s="9"/>
-      <c r="E521" s="2"/>
+      <c r="A521" s="21" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B521" s="22">
+        <v>461</v>
+      </c>
+      <c r="C521" s="22">
+        <v>0</v>
+      </c>
+      <c r="D521" s="22">
+        <v>216</v>
+      </c>
+      <c r="E521" s="23" t="s">
+        <v>1058</v>
+      </c>
     </row>
     <row r="522" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A522" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B522" s="9"/>
-      <c r="C522" s="9"/>
-      <c r="D522" s="9"/>
-      <c r="E522" s="2"/>
+      <c r="A522" s="21" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B522" s="22">
+        <v>596</v>
+      </c>
+      <c r="C522" s="22">
+        <v>0</v>
+      </c>
+      <c r="D522" s="22">
+        <v>0</v>
+      </c>
+      <c r="E522" s="23" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="523" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A523" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B523" s="9"/>
-      <c r="C523" s="9"/>
-      <c r="D523" s="9"/>
-      <c r="E523" s="2"/>
+      <c r="A523" s="21" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B523" s="22">
+        <v>504</v>
+      </c>
+      <c r="C523" s="22">
+        <v>2</v>
+      </c>
+      <c r="D523" s="22">
+        <v>55</v>
+      </c>
+      <c r="E523" s="23" t="s">
+        <v>1060</v>
+      </c>
     </row>
     <row r="524" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A524" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B524" s="9"/>
-      <c r="C524" s="9"/>
-      <c r="D524" s="9"/>
-      <c r="E524" s="2"/>
+      <c r="A524" s="21" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B524" s="22">
+        <v>618</v>
+      </c>
+      <c r="C524" s="22">
+        <v>0</v>
+      </c>
+      <c r="D524" s="22">
+        <v>60</v>
+      </c>
+      <c r="E524" s="23" t="s">
+        <v>1061</v>
+      </c>
     </row>
     <row r="525" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A525" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B525" s="9"/>
-      <c r="C525" s="9"/>
-      <c r="D525" s="9"/>
-      <c r="E525" s="2"/>
-    </row>
-    <row r="526" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A526" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B526" s="9"/>
-      <c r="C526" s="9"/>
-      <c r="D526" s="9"/>
-      <c r="E526" s="2"/>
+      <c r="A525" s="21" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B525" s="22">
+        <v>406</v>
+      </c>
+      <c r="C525" s="22">
+        <v>0</v>
+      </c>
+      <c r="D525" s="22">
+        <v>30</v>
+      </c>
+      <c r="E525" s="23" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A526" s="21" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B526" s="22">
+        <v>612</v>
+      </c>
+      <c r="C526" s="22">
+        <v>0</v>
+      </c>
+      <c r="D526" s="22">
+        <v>69</v>
+      </c>
+      <c r="E526" s="23" t="s">
+        <v>1063</v>
+      </c>
     </row>
     <row r="527" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A527" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B527" s="9"/>
-      <c r="C527" s="9"/>
-      <c r="D527" s="9"/>
-      <c r="E527" s="2"/>
+      <c r="A527" s="21" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B527" s="22">
+        <v>628</v>
+      </c>
+      <c r="C527" s="22">
+        <v>0</v>
+      </c>
+      <c r="D527" s="22">
+        <v>29</v>
+      </c>
+      <c r="E527" s="23" t="s">
+        <v>1064</v>
+      </c>
     </row>
     <row r="528" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A528" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B528" s="9"/>
-      <c r="C528" s="9"/>
-      <c r="D528" s="9"/>
-      <c r="E528" s="2"/>
-    </row>
-    <row r="529" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A529" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B529" s="9"/>
-      <c r="C529" s="9"/>
-      <c r="D529" s="9"/>
-      <c r="E529" s="2"/>
+      <c r="A528" s="21" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B528" s="22">
+        <v>592</v>
+      </c>
+      <c r="C528" s="22">
+        <v>0</v>
+      </c>
+      <c r="D528" s="22">
+        <v>47</v>
+      </c>
+      <c r="E528" s="23" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A529" s="21" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B529" s="22">
+        <v>688</v>
+      </c>
+      <c r="C529" s="22">
+        <v>2</v>
+      </c>
+      <c r="D529" s="22">
+        <v>6</v>
+      </c>
+      <c r="E529" s="23" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="530" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A530" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B530" s="9"/>
-      <c r="C530" s="9"/>
-      <c r="D530" s="9"/>
-      <c r="E530" s="2"/>
+      <c r="A530" s="21" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B530" s="22">
+        <v>622</v>
+      </c>
+      <c r="C530" s="22">
+        <v>0</v>
+      </c>
+      <c r="D530" s="22">
+        <v>4</v>
+      </c>
+      <c r="E530" s="23" t="s">
+        <v>1071</v>
+      </c>
     </row>
     <row r="531" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A531" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B531" s="9"/>
-      <c r="C531" s="9"/>
-      <c r="D531" s="9"/>
-      <c r="E531" s="2"/>
+      <c r="A531" s="21" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B531" s="22">
+        <v>793</v>
+      </c>
+      <c r="C531" s="22">
+        <v>0</v>
+      </c>
+      <c r="D531" s="22">
+        <v>114</v>
+      </c>
+      <c r="E531" s="23" t="s">
+        <v>1072</v>
+      </c>
     </row>
     <row r="532" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A532" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B532" s="9"/>
-      <c r="C532" s="9"/>
-      <c r="D532" s="9"/>
-      <c r="E532" s="2"/>
+      <c r="A532" s="21" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B532" s="22">
+        <v>830</v>
+      </c>
+      <c r="C532" s="22">
+        <v>0</v>
+      </c>
+      <c r="D532" s="22">
+        <v>94</v>
+      </c>
+      <c r="E532" s="23" t="s">
+        <v>1073</v>
+      </c>
     </row>
     <row r="533" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A533" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B533" s="9"/>
-      <c r="C533" s="9"/>
-      <c r="D533" s="9"/>
-      <c r="E533" s="2"/>
+      <c r="A533" s="21" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B533" s="22">
+        <v>592</v>
+      </c>
+      <c r="C533" s="22">
+        <v>0</v>
+      </c>
+      <c r="D533" s="22">
+        <v>20</v>
+      </c>
+      <c r="E533" s="23" t="s">
+        <v>1067</v>
+      </c>
     </row>
     <row r="534" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A534" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B534" s="9"/>
-      <c r="C534" s="9"/>
-      <c r="D534" s="9"/>
-      <c r="E534" s="2"/>
+      <c r="A534" s="21" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B534" s="22">
+        <v>811</v>
+      </c>
+      <c r="C534" s="22">
+        <v>0</v>
+      </c>
+      <c r="D534" s="22">
+        <v>45</v>
+      </c>
+      <c r="E534" s="23" t="s">
+        <v>1068</v>
+      </c>
     </row>
     <row r="535" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A535" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B535" s="9"/>
-      <c r="C535" s="9"/>
-      <c r="D535" s="9"/>
-      <c r="E535" s="2"/>
+      <c r="A535" s="21" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B535" s="22">
+        <v>858</v>
+      </c>
+      <c r="C535" s="22">
+        <v>0</v>
+      </c>
+      <c r="D535" s="22">
+        <v>42</v>
+      </c>
+      <c r="E535" s="23" t="s">
+        <v>1069</v>
+      </c>
     </row>
     <row r="536" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A536" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B536" s="9"/>
-      <c r="C536" s="9"/>
-      <c r="D536" s="9"/>
-      <c r="E536" s="2"/>
+      <c r="A536" s="21" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B536" s="22">
+        <v>851</v>
+      </c>
+      <c r="C536" s="22">
+        <v>2</v>
+      </c>
+      <c r="D536" s="22">
+        <v>33</v>
+      </c>
+      <c r="E536" s="23" t="s">
+        <v>1070</v>
+      </c>
     </row>
     <row r="537" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A537" s="10" t="s">

</xml_diff>

<commit_message>
songlist update DLC #5
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25DFA0B-C100-4A5E-AE1B-B38FAE0A74AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C3A36-35B6-454F-96C6-5ED69007498C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="1211">
   <si>
     <t>Rapid Fire (SH 7)</t>
   </si>
@@ -3466,13 +3466,214 @@
   </si>
   <si>
     <t>Throne (SX 14)</t>
+  </si>
+  <si>
+    <t>Underwater Regret (SH)</t>
+  </si>
+  <si>
+    <t>Fluxillary (SH)</t>
+  </si>
+  <si>
+    <t>Hakken (SM)</t>
+  </si>
+  <si>
+    <t>Johnny's Got That Funk (SH)</t>
+  </si>
+  <si>
+    <t>Push the Fader (SH)</t>
+  </si>
+  <si>
+    <t>Arcade</t>
+  </si>
+  <si>
+    <t>Multitalents (SM)</t>
+  </si>
+  <si>
+    <t>subtractive (SH)</t>
+  </si>
+  <si>
+    <t>Remix 1</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Bass in Da House</t>
+  </si>
+  <si>
+    <t>Big Phil</t>
+  </si>
+  <si>
+    <t>DeltaMax</t>
+  </si>
+  <si>
+    <t>Fluxillary</t>
+  </si>
+  <si>
+    <t>mavepine</t>
+  </si>
+  <si>
+    <t>Throw your cards down (Nhato remix)</t>
+  </si>
+  <si>
+    <t>Abyss</t>
+  </si>
+  <si>
+    <t>Bassline &amp; Sexy</t>
+  </si>
+  <si>
+    <t>Fracture Ray</t>
+  </si>
+  <si>
+    <t>MASAMUNE</t>
+  </si>
+  <si>
+    <t>Super Reactor</t>
+  </si>
+  <si>
+    <t>Young Killa</t>
+  </si>
+  <si>
+    <t>Harpoon</t>
+  </si>
+  <si>
+    <t>Hysteria</t>
+  </si>
+  <si>
+    <t>imissu My Fine Neko Shot Sunrise</t>
+  </si>
+  <si>
+    <t>Paradoxy (Camellia's "PERPETUAL" remix)</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Eg0 (SE)</t>
+  </si>
+  <si>
+    <t>GIGA VIOLATE</t>
+  </si>
+  <si>
+    <t>Palpitation</t>
+  </si>
+  <si>
+    <t>Sudden Visitor</t>
+  </si>
+  <si>
+    <t>Super Hyper Miracle Fantasy Parade</t>
+  </si>
+  <si>
+    <t>Windy Windy Wind</t>
+  </si>
+  <si>
+    <t>Underwater Regret (SH 7)</t>
+  </si>
+  <si>
+    <t>Fluxillary (SH 8)</t>
+  </si>
+  <si>
+    <t>Hakken (SM 8)</t>
+  </si>
+  <si>
+    <t>Johnny's Got That Funk (SH 8)</t>
+  </si>
+  <si>
+    <t>Push The Fader (SH 8)</t>
+  </si>
+  <si>
+    <t>Arcade (SX 9)</t>
+  </si>
+  <si>
+    <t>Multitalents (SM 9)</t>
+  </si>
+  <si>
+    <t>subtractive (SH 9)</t>
+  </si>
+  <si>
+    <t>Remix 1 (SX 10)</t>
+  </si>
+  <si>
+    <t>Shoes (Club Fantastic Edit) (SX 10)</t>
+  </si>
+  <si>
+    <t>Bass In Da House (SX 11)</t>
+  </si>
+  <si>
+    <t>Big Phil (SX 11)</t>
+  </si>
+  <si>
+    <t>DeltaMAX (SM 11)</t>
+  </si>
+  <si>
+    <t>Fluxillary (SX 11)</t>
+  </si>
+  <si>
+    <t>mavepine (SX 11)</t>
+  </si>
+  <si>
+    <t>Throw your cards down (Nhato Remix) (SX 11)</t>
+  </si>
+  <si>
+    <t>Abyss (SX 12)</t>
+  </si>
+  <si>
+    <t>Bassline &amp; Sexy (Original Mix) (SX 12)</t>
+  </si>
+  <si>
+    <t>Fracture Ray (SX 12)</t>
+  </si>
+  <si>
+    <t>MASAMUNE (SX 12)</t>
+  </si>
+  <si>
+    <t>SUPER REACTOR (SX 12)</t>
+  </si>
+  <si>
+    <t>Young Killa (SX 12)</t>
+  </si>
+  <si>
+    <t>Harpoon (SX 13)</t>
+  </si>
+  <si>
+    <t>hysteria (SX 13)</t>
+  </si>
+  <si>
+    <t>imissu My Fine Neko Shot Sunrise (SX 13)</t>
+  </si>
+  <si>
+    <t>Paradoxy (Camellia's PERPETUAL Remix) (SX 13)</t>
+  </si>
+  <si>
+    <t>Radius (SX 13)</t>
+  </si>
+  <si>
+    <t>EgO (SE 14)</t>
+  </si>
+  <si>
+    <t>GIGA VIOLATE (SX 14)</t>
+  </si>
+  <si>
+    <t>I (SX 14)</t>
+  </si>
+  <si>
+    <t>Palpitation (SX 14)</t>
+  </si>
+  <si>
+    <t>Sudden Visitor (SX 14)</t>
+  </si>
+  <si>
+    <t>SUPER HYPER MIRACLE FANTASY PARADE (SX 14)</t>
+  </si>
+  <si>
+    <t>Windy Windy Wind (SX 14)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3521,8 +3722,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3556,6 +3770,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCFEAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3647,7 +3873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3727,6 +3953,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4047,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
-  <dimension ref="A1:E607"/>
+  <dimension ref="A1:E630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A551" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E567" sqref="E567:E572"/>
+    <sheetView tabSelected="1" topLeftCell="A590" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E600" sqref="E600:E606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13786,319 +14024,775 @@
       </c>
     </row>
     <row r="573" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A573" s="6" t="s">
+      <c r="A573" s="28" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B573" s="29">
+        <v>369</v>
+      </c>
+      <c r="C573" s="29">
+        <v>0</v>
+      </c>
+      <c r="D573" s="29">
+        <v>46</v>
+      </c>
+      <c r="E573" s="28" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A574" s="28" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B574" s="29">
+        <v>333</v>
+      </c>
+      <c r="C574" s="29">
+        <v>8</v>
+      </c>
+      <c r="D574" s="29">
+        <v>33</v>
+      </c>
+      <c r="E574" s="28" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A575" s="28" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B575" s="29">
+        <v>365</v>
+      </c>
+      <c r="C575" s="29">
+        <v>6</v>
+      </c>
+      <c r="D575" s="29">
+        <v>43</v>
+      </c>
+      <c r="E575" s="28" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A576" s="28" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B576" s="29">
+        <v>362</v>
+      </c>
+      <c r="C576" s="29">
+        <v>13</v>
+      </c>
+      <c r="D576" s="29">
+        <v>18</v>
+      </c>
+      <c r="E576" s="28" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A577" s="28" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B577" s="29">
+        <v>454</v>
+      </c>
+      <c r="C577" s="29">
+        <v>1</v>
+      </c>
+      <c r="D577" s="29">
+        <v>40</v>
+      </c>
+      <c r="E577" s="28" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A578" s="28" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B578" s="29">
+        <v>436</v>
+      </c>
+      <c r="C578" s="29">
+        <v>1</v>
+      </c>
+      <c r="D578" s="29">
+        <v>77</v>
+      </c>
+      <c r="E578" s="28" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A579" s="28" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B579" s="29">
+        <v>536</v>
+      </c>
+      <c r="C579" s="29">
+        <v>9</v>
+      </c>
+      <c r="D579" s="29">
+        <v>30</v>
+      </c>
+      <c r="E579" s="28" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A580" s="28" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B580" s="29">
+        <v>579</v>
+      </c>
+      <c r="C580" s="29">
+        <v>13</v>
+      </c>
+      <c r="D580" s="29">
+        <v>21</v>
+      </c>
+      <c r="E580" s="28" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="581" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A581" s="28" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B581" s="29">
+        <v>470</v>
+      </c>
+      <c r="C581" s="29">
+        <v>2</v>
+      </c>
+      <c r="D581" s="29">
+        <v>37</v>
+      </c>
+      <c r="E581" s="28" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="582" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A582" s="28" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B582" s="29">
+        <v>475</v>
+      </c>
+      <c r="C582" s="29">
+        <v>0</v>
+      </c>
+      <c r="D582" s="29">
+        <v>49</v>
+      </c>
+      <c r="E582" s="28" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="583" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A583" s="28" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B583" s="29">
+        <v>605</v>
+      </c>
+      <c r="C583" s="29">
+        <v>4</v>
+      </c>
+      <c r="D583" s="29">
+        <v>80</v>
+      </c>
+      <c r="E583" s="28" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="584" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A584" s="28" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B584" s="29">
+        <v>551</v>
+      </c>
+      <c r="C584" s="29">
+        <v>2</v>
+      </c>
+      <c r="D584" s="29">
+        <v>8</v>
+      </c>
+      <c r="E584" s="28" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="585" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A585" s="28" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B585" s="29">
+        <v>604</v>
+      </c>
+      <c r="C585" s="29">
+        <v>0</v>
+      </c>
+      <c r="D585" s="29">
+        <v>3</v>
+      </c>
+      <c r="E585" s="28" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="586" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A586" s="28" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B586" s="29">
+        <v>510</v>
+      </c>
+      <c r="C586" s="29">
+        <v>6</v>
+      </c>
+      <c r="D586" s="29">
+        <v>46</v>
+      </c>
+      <c r="E586" s="28" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="587" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A587" s="28" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B587" s="29">
+        <v>558</v>
+      </c>
+      <c r="C587" s="29">
+        <v>0</v>
+      </c>
+      <c r="D587" s="29">
+        <v>43</v>
+      </c>
+      <c r="E587" s="28" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A588" s="28" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B588" s="29">
+        <v>674</v>
+      </c>
+      <c r="C588" s="29">
+        <v>0</v>
+      </c>
+      <c r="D588" s="29">
+        <v>49</v>
+      </c>
+      <c r="E588" s="28" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A589" s="28" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B589" s="29">
+        <v>783</v>
+      </c>
+      <c r="C589" s="29">
+        <v>2</v>
+      </c>
+      <c r="D589" s="29">
+        <v>94</v>
+      </c>
+      <c r="E589" s="28" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="590" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A590" s="28" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B590" s="29">
+        <v>702</v>
+      </c>
+      <c r="C590" s="29">
+        <v>73</v>
+      </c>
+      <c r="D590" s="29">
+        <v>39</v>
+      </c>
+      <c r="E590" s="28" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="591" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A591" s="28" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B591" s="29">
+        <v>633</v>
+      </c>
+      <c r="C591" s="29">
+        <v>11</v>
+      </c>
+      <c r="D591" s="29">
+        <v>57</v>
+      </c>
+      <c r="E591" s="28" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="592" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A592" s="28" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B592" s="29">
+        <v>805</v>
+      </c>
+      <c r="C592" s="29">
+        <v>1</v>
+      </c>
+      <c r="D592" s="29">
+        <v>34</v>
+      </c>
+      <c r="E592" s="28" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="593" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A593" s="28" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B593" s="29">
+        <v>833</v>
+      </c>
+      <c r="C593" s="29">
+        <v>4</v>
+      </c>
+      <c r="D593" s="29">
+        <v>75</v>
+      </c>
+      <c r="E593" s="28" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="594" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A594" s="28" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B594" s="29">
+        <v>607</v>
+      </c>
+      <c r="C594" s="29">
+        <v>17</v>
+      </c>
+      <c r="D594" s="29">
+        <v>35</v>
+      </c>
+      <c r="E594" s="28" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A595" s="28" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B595" s="29">
+        <v>826</v>
+      </c>
+      <c r="C595" s="29">
+        <v>0</v>
+      </c>
+      <c r="D595" s="29">
+        <v>14</v>
+      </c>
+      <c r="E595" s="28" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="596" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A596" s="28" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B596" s="29">
+        <v>816</v>
+      </c>
+      <c r="C596" s="29">
+        <v>0</v>
+      </c>
+      <c r="D596" s="29">
+        <v>80</v>
+      </c>
+      <c r="E596" s="28" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A597" s="28" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B597" s="29">
+        <v>1601</v>
+      </c>
+      <c r="C597" s="29">
+        <v>6</v>
+      </c>
+      <c r="D597" s="29">
+        <v>48</v>
+      </c>
+      <c r="E597" s="28" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A598" s="28" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B598" s="29">
+        <v>932</v>
+      </c>
+      <c r="C598" s="29">
+        <v>29</v>
+      </c>
+      <c r="D598" s="29">
+        <v>109</v>
+      </c>
+      <c r="E598" s="28" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A599" s="28" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B599" s="29">
+        <v>741</v>
+      </c>
+      <c r="C599" s="29">
+        <v>1</v>
+      </c>
+      <c r="D599" s="29">
+        <v>103</v>
+      </c>
+      <c r="E599" s="28" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A600" s="28" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B600" s="29">
+        <v>1029</v>
+      </c>
+      <c r="C600" s="29">
+        <v>0</v>
+      </c>
+      <c r="D600" s="29">
+        <v>81</v>
+      </c>
+      <c r="E600" s="28" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A601" s="28" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B601" s="29">
+        <v>880</v>
+      </c>
+      <c r="C601" s="29">
+        <v>5</v>
+      </c>
+      <c r="D601" s="29">
+        <v>47</v>
+      </c>
+      <c r="E601" s="28" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A602" s="28" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B602" s="29">
+        <v>922</v>
+      </c>
+      <c r="C602" s="29">
+        <v>26</v>
+      </c>
+      <c r="D602" s="29">
+        <v>33</v>
+      </c>
+      <c r="E602" s="28" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="603" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A603" s="28" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B603" s="29">
+        <v>777</v>
+      </c>
+      <c r="C603" s="29">
+        <v>6</v>
+      </c>
+      <c r="D603" s="29">
+        <v>98</v>
+      </c>
+      <c r="E603" s="28" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A604" s="28" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B604" s="29">
+        <v>1095</v>
+      </c>
+      <c r="C604" s="29">
+        <v>1</v>
+      </c>
+      <c r="D604" s="29">
+        <v>138</v>
+      </c>
+      <c r="E604" s="28" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="605" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A605" s="28" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B605" s="29">
+        <v>1110</v>
+      </c>
+      <c r="C605" s="29">
+        <v>9</v>
+      </c>
+      <c r="D605" s="29">
+        <v>88</v>
+      </c>
+      <c r="E605" s="28" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A606" s="28" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B606" s="29">
+        <v>852</v>
+      </c>
+      <c r="C606" s="29">
+        <v>0</v>
+      </c>
+      <c r="D606" s="29">
+        <v>7</v>
+      </c>
+      <c r="E606" s="28" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A607" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B573" s="5"/>
-      <c r="C573" s="5"/>
-      <c r="D573" s="5"/>
-      <c r="E573" s="21"/>
-    </row>
-    <row r="574" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A574" s="6" t="s">
+      <c r="B607" s="31"/>
+      <c r="C607" s="31"/>
+      <c r="D607" s="31"/>
+      <c r="E607" s="21"/>
+    </row>
+    <row r="608" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A608" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B574" s="5"/>
-      <c r="C574" s="5"/>
-      <c r="D574" s="5"/>
-      <c r="E574" s="21"/>
-    </row>
-    <row r="575" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A575" s="6" t="s">
+      <c r="B608" s="31"/>
+      <c r="C608" s="31"/>
+      <c r="D608" s="31"/>
+    </row>
+    <row r="609" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A609" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B575" s="5"/>
-      <c r="C575" s="5"/>
-      <c r="D575" s="5"/>
-      <c r="E575" s="21"/>
-    </row>
-    <row r="576" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A576" s="6" t="s">
+      <c r="B609" s="31"/>
+      <c r="C609" s="31"/>
+      <c r="D609" s="31"/>
+    </row>
+    <row r="610" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A610" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B576" s="5"/>
-      <c r="C576" s="5"/>
-      <c r="D576" s="5"/>
-      <c r="E576" s="21"/>
-    </row>
-    <row r="577" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A577" s="6" t="s">
+      <c r="B610" s="31"/>
+      <c r="C610" s="31"/>
+      <c r="D610" s="31"/>
+    </row>
+    <row r="611" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A611" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B577" s="5"/>
-      <c r="C577" s="5"/>
-      <c r="D577" s="5"/>
-      <c r="E577" s="21"/>
-    </row>
-    <row r="578" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A578" s="6" t="s">
+      <c r="B611" s="31"/>
+      <c r="C611" s="31"/>
+      <c r="D611" s="31"/>
+    </row>
+    <row r="612" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A612" s="30" t="s">
         <v>483</v>
       </c>
-      <c r="B578" s="5"/>
-      <c r="C578" s="5"/>
-      <c r="D578" s="5"/>
-      <c r="E578" s="21"/>
-    </row>
-    <row r="579" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A579" s="6" t="s">
+      <c r="B612" s="31"/>
+      <c r="C612" s="31"/>
+      <c r="D612" s="31"/>
+    </row>
+    <row r="613" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A613" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B579" s="5"/>
-      <c r="C579" s="5"/>
-      <c r="D579" s="5"/>
-      <c r="E579" s="21"/>
-    </row>
-    <row r="580" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A580" s="6" t="s">
+      <c r="B613" s="5"/>
+      <c r="C613" s="5"/>
+      <c r="D613" s="5"/>
+    </row>
+    <row r="614" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A614" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B580" s="5"/>
-      <c r="C580" s="5"/>
-      <c r="D580" s="5"/>
-      <c r="E580" s="21"/>
-    </row>
-    <row r="581" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A581" s="6" t="s">
+      <c r="B614" s="5"/>
+      <c r="C614" s="5"/>
+      <c r="D614" s="5"/>
+    </row>
+    <row r="615" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A615" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B581" s="5"/>
-      <c r="C581" s="5"/>
-      <c r="D581" s="5"/>
-      <c r="E581" s="21"/>
-    </row>
-    <row r="582" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A582" s="6" t="s">
+      <c r="B615" s="5"/>
+      <c r="C615" s="5"/>
+      <c r="D615" s="5"/>
+    </row>
+    <row r="616" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A616" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B582" s="5"/>
-      <c r="C582" s="5"/>
-      <c r="D582" s="5"/>
-      <c r="E582" s="21"/>
-    </row>
-    <row r="583" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A583" s="6" t="s">
+      <c r="B616" s="5"/>
+      <c r="C616" s="5"/>
+      <c r="D616" s="5"/>
+    </row>
+    <row r="617" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A617" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B583" s="5"/>
-      <c r="C583" s="5"/>
-      <c r="D583" s="5"/>
-      <c r="E583" s="21"/>
-    </row>
-    <row r="584" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A584" s="6" t="s">
+      <c r="B617" s="5"/>
+      <c r="C617" s="5"/>
+      <c r="D617" s="5"/>
+    </row>
+    <row r="618" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A618" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B584" s="5"/>
-      <c r="C584" s="5"/>
-      <c r="D584" s="5"/>
-      <c r="E584" s="21"/>
-    </row>
-    <row r="585" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A585" s="6" t="s">
+      <c r="B618" s="5"/>
+      <c r="C618" s="5"/>
+      <c r="D618" s="5"/>
+    </row>
+    <row r="619" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A619" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B585" s="5"/>
-      <c r="C585" s="5"/>
-      <c r="D585" s="5"/>
-      <c r="E585" s="21"/>
-    </row>
-    <row r="586" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A586" s="6" t="s">
+      <c r="B619" s="5"/>
+      <c r="C619" s="5"/>
+      <c r="D619" s="5"/>
+    </row>
+    <row r="620" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A620" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B586" s="5"/>
-      <c r="C586" s="5"/>
-      <c r="D586" s="5"/>
-      <c r="E586" s="21"/>
-    </row>
-    <row r="587" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A587" s="6" t="s">
+      <c r="B620" s="5"/>
+      <c r="C620" s="5"/>
+      <c r="D620" s="5"/>
+    </row>
+    <row r="621" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A621" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B587" s="5"/>
-      <c r="C587" s="5"/>
-      <c r="D587" s="5"/>
-      <c r="E587" s="21"/>
-    </row>
-    <row r="588" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A588" s="6" t="s">
+      <c r="B621" s="5"/>
+      <c r="C621" s="5"/>
+      <c r="D621" s="5"/>
+    </row>
+    <row r="622" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A622" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B588" s="5"/>
-      <c r="C588" s="5"/>
-      <c r="D588" s="5"/>
-      <c r="E588" s="21"/>
-    </row>
-    <row r="589" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A589" s="6" t="s">
+      <c r="B622" s="5"/>
+      <c r="C622" s="5"/>
+      <c r="D622" s="5"/>
+    </row>
+    <row r="623" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A623" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B589" s="5"/>
-      <c r="C589" s="5"/>
-      <c r="D589" s="5"/>
-      <c r="E589" s="21"/>
-    </row>
-    <row r="590" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A590" s="6" t="s">
+      <c r="B623" s="5"/>
+      <c r="C623" s="5"/>
+      <c r="D623" s="5"/>
+    </row>
+    <row r="624" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A624" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B590" s="5"/>
-      <c r="C590" s="5"/>
-      <c r="D590" s="5"/>
-      <c r="E590" s="21"/>
-    </row>
-    <row r="591" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A591" s="6" t="s">
+      <c r="B624" s="5"/>
+      <c r="C624" s="5"/>
+      <c r="D624" s="5"/>
+    </row>
+    <row r="625" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A625" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B591" s="5"/>
-      <c r="C591" s="5"/>
-      <c r="D591" s="5"/>
-      <c r="E591" s="21"/>
-    </row>
-    <row r="592" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A592" s="6" t="s">
+      <c r="B625" s="5"/>
+      <c r="C625" s="5"/>
+      <c r="D625" s="5"/>
+    </row>
+    <row r="626" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A626" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B592" s="5"/>
-      <c r="C592" s="5"/>
-      <c r="D592" s="5"/>
-      <c r="E592" s="21"/>
-    </row>
-    <row r="593" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A593" s="6" t="s">
+      <c r="B626" s="5"/>
+      <c r="C626" s="5"/>
+      <c r="D626" s="5"/>
+    </row>
+    <row r="627" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A627" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B593" s="5"/>
-      <c r="C593" s="5"/>
-      <c r="D593" s="5"/>
-      <c r="E593" s="21"/>
-    </row>
-    <row r="594" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A594" s="6" t="s">
+      <c r="B627" s="5"/>
+      <c r="C627" s="5"/>
+      <c r="D627" s="5"/>
+    </row>
+    <row r="628" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A628" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B594" s="5"/>
-      <c r="C594" s="5"/>
-      <c r="D594" s="5"/>
-      <c r="E594" s="21"/>
-    </row>
-    <row r="595" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A595" s="6" t="s">
+      <c r="B628" s="5"/>
+      <c r="C628" s="5"/>
+      <c r="D628" s="5"/>
+    </row>
+    <row r="629" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A629" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B595" s="5"/>
-      <c r="C595" s="5"/>
-      <c r="D595" s="5"/>
-      <c r="E595" s="21"/>
-    </row>
-    <row r="596" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A596" s="6" t="s">
+      <c r="B629" s="5"/>
+      <c r="C629" s="5"/>
+      <c r="D629" s="5"/>
+    </row>
+    <row r="630" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A630" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="B596" s="5"/>
-      <c r="C596" s="5"/>
-      <c r="D596" s="5"/>
-      <c r="E596" s="21"/>
-    </row>
-    <row r="597" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A597" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B597" s="5"/>
-      <c r="C597" s="5"/>
-      <c r="D597" s="5"/>
-      <c r="E597" s="21"/>
-    </row>
-    <row r="598" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A598" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B598" s="5"/>
-      <c r="C598" s="5"/>
-      <c r="D598" s="5"/>
-      <c r="E598" s="21"/>
-    </row>
-    <row r="599" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A599" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B599" s="5"/>
-      <c r="C599" s="5"/>
-      <c r="D599" s="5"/>
-      <c r="E599" s="21"/>
-    </row>
-    <row r="600" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A600" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B600" s="5"/>
-      <c r="C600" s="5"/>
-      <c r="D600" s="5"/>
-      <c r="E600" s="21"/>
-    </row>
-    <row r="601" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A601" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B601" s="5"/>
-      <c r="C601" s="5"/>
-      <c r="D601" s="5"/>
-      <c r="E601" s="21"/>
-    </row>
-    <row r="602" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A602" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B602" s="5"/>
-      <c r="C602" s="5"/>
-      <c r="D602" s="5"/>
-      <c r="E602" s="21"/>
-    </row>
-    <row r="603" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A603" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B603" s="5"/>
-      <c r="C603" s="5"/>
-      <c r="D603" s="5"/>
-      <c r="E603" s="21"/>
-    </row>
-    <row r="604" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A604" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B604" s="5"/>
-      <c r="C604" s="5"/>
-      <c r="D604" s="5"/>
-      <c r="E604" s="21"/>
-    </row>
-    <row r="605" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A605" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B605" s="5"/>
-      <c r="C605" s="5"/>
-      <c r="D605" s="5"/>
-      <c r="E605" s="21"/>
-    </row>
-    <row r="606" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A606" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B606" s="5"/>
-      <c r="C606" s="5"/>
-      <c r="D606" s="5"/>
-      <c r="E606" s="21"/>
-    </row>
-    <row r="607" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A607" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B607" s="5"/>
-      <c r="C607" s="5"/>
-      <c r="D607" s="5"/>
-      <c r="E607" s="21"/>
+      <c r="B630" s="5"/>
+      <c r="C630" s="5"/>
+      <c r="D630" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix stepcount on Vector Field
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C3A36-35B6-454F-96C6-5ED69007498C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B562980F-F39D-4A58-A457-8049B81CC0D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -4287,8 +4287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
   <dimension ref="A1:E630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A590" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E600" sqref="E600:E606"/>
+    <sheetView tabSelected="1" topLeftCell="A500" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B513" sqref="B513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13008,7 +13008,7 @@
         <v>992</v>
       </c>
       <c r="B513" s="13">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="C513" s="13">
         <v>2</v>

</xml_diff>

<commit_message>
update songlist.json for Boss Pack #1 and #2
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\source\repos\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B562980F-F39D-4A58-A457-8049B81CC0D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7A4511-540C-4E4C-AEBB-CC2B4A30FB9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="1235">
   <si>
     <t>Rapid Fire (SH 7)</t>
   </si>
@@ -3667,6 +3667,78 @@
   </si>
   <si>
     <t>Windy Windy Wind (SX 14)</t>
+  </si>
+  <si>
+    <t>Chatterbox</t>
+  </si>
+  <si>
+    <t>Knots</t>
+  </si>
+  <si>
+    <t>Critical Crystal (brz remix)</t>
+  </si>
+  <si>
+    <t>Turning Point</t>
+  </si>
+  <si>
+    <t>PP is Dead</t>
+  </si>
+  <si>
+    <t>Prime Time</t>
+  </si>
+  <si>
+    <t>Sweet Devil SketchP remix</t>
+  </si>
+  <si>
+    <t>Jam Jam Reggae</t>
+  </si>
+  <si>
+    <t>Fat Controller</t>
+  </si>
+  <si>
+    <t>corps-sans-organes</t>
+  </si>
+  <si>
+    <t>Estrangement</t>
+  </si>
+  <si>
+    <t>Dyscontrolled Galaxy</t>
+  </si>
+  <si>
+    <t>Sweet Devil (SketchP Remix)</t>
+  </si>
+  <si>
+    <t>Jam Jam Reggae (AMD Swing Mix) (SX 10)</t>
+  </si>
+  <si>
+    <t>Fat Controller (SX 11)</t>
+  </si>
+  <si>
+    <t>corps-sans-organes (SX 12)</t>
+  </si>
+  <si>
+    <t>Estrangement (SX 13)</t>
+  </si>
+  <si>
+    <t>Dyscontrolled Galaxy (SX 14)</t>
+  </si>
+  <si>
+    <t>Chatterbox (SX 9)</t>
+  </si>
+  <si>
+    <t>Knots (SX 10)</t>
+  </si>
+  <si>
+    <t>Critical Crystal (brz_remix) (SX 11)</t>
+  </si>
+  <si>
+    <t>Turning Point (SX 12)</t>
+  </si>
+  <si>
+    <t>PP is Dead (SX 13)</t>
+  </si>
+  <si>
+    <t>Prime Time (SX 14)</t>
   </si>
 </sst>
 </file>
@@ -3730,13 +3802,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00FFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3782,6 +3855,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF910000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3873,7 +3952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3963,8 +4042,20 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4287,8 +4378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
   <dimension ref="A1:E630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A500" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B513" sqref="B513"/>
+    <sheetView tabSelected="1" topLeftCell="A602" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E608" sqref="E608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14603,102 +14694,209 @@
     </row>
     <row r="607" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A607" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B607" s="31"/>
-      <c r="C607" s="31"/>
-      <c r="D607" s="31"/>
-      <c r="E607" s="21"/>
+        <v>1211</v>
+      </c>
+      <c r="B607" s="31">
+        <v>507</v>
+      </c>
+      <c r="C607" s="31">
+        <v>4</v>
+      </c>
+      <c r="D607" s="31">
+        <v>74</v>
+      </c>
+      <c r="E607" s="34" t="s">
+        <v>1229</v>
+      </c>
     </row>
     <row r="608" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A608" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B608" s="31"/>
-      <c r="C608" s="31"/>
-      <c r="D608" s="31"/>
-    </row>
-    <row r="609" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1212</v>
+      </c>
+      <c r="B608" s="31">
+        <v>565</v>
+      </c>
+      <c r="C608" s="31">
+        <v>11</v>
+      </c>
+      <c r="D608" s="31">
+        <v>37</v>
+      </c>
+      <c r="E608" s="34" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="609" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A609" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B609" s="31"/>
-      <c r="C609" s="31"/>
-      <c r="D609" s="31"/>
-    </row>
-    <row r="610" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1213</v>
+      </c>
+      <c r="B609" s="31">
+        <v>653</v>
+      </c>
+      <c r="C609" s="31">
+        <v>0</v>
+      </c>
+      <c r="D609" s="31">
+        <v>49</v>
+      </c>
+      <c r="E609" s="34" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="610" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A610" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B610" s="31"/>
-      <c r="C610" s="31"/>
-      <c r="D610" s="31"/>
-    </row>
-    <row r="611" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1214</v>
+      </c>
+      <c r="B610" s="31">
+        <v>895</v>
+      </c>
+      <c r="C610" s="31">
+        <v>12</v>
+      </c>
+      <c r="D610" s="31">
+        <v>42</v>
+      </c>
+      <c r="E610" s="34" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="611" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A611" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B611" s="31"/>
-      <c r="C611" s="31"/>
-      <c r="D611" s="31"/>
-    </row>
-    <row r="612" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1215</v>
+      </c>
+      <c r="B611" s="31">
+        <v>659</v>
+      </c>
+      <c r="C611" s="31">
+        <v>0</v>
+      </c>
+      <c r="D611" s="31">
+        <v>118</v>
+      </c>
+      <c r="E611" s="34" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="612" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A612" s="30" t="s">
-        <v>483</v>
-      </c>
-      <c r="B612" s="31"/>
-      <c r="C612" s="31"/>
-      <c r="D612" s="31"/>
-    </row>
-    <row r="613" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A613" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B613" s="5"/>
-      <c r="C613" s="5"/>
-      <c r="D613" s="5"/>
-    </row>
-    <row r="614" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A614" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B614" s="5"/>
-      <c r="C614" s="5"/>
-      <c r="D614" s="5"/>
-    </row>
-    <row r="615" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A615" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B615" s="5"/>
-      <c r="C615" s="5"/>
-      <c r="D615" s="5"/>
-    </row>
-    <row r="616" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A616" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B616" s="5"/>
-      <c r="C616" s="5"/>
-      <c r="D616" s="5"/>
-    </row>
-    <row r="617" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A617" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B617" s="5"/>
-      <c r="C617" s="5"/>
-      <c r="D617" s="5"/>
-    </row>
-    <row r="618" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A618" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B618" s="5"/>
-      <c r="C618" s="5"/>
-      <c r="D618" s="5"/>
-    </row>
-    <row r="619" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1216</v>
+      </c>
+      <c r="B612" s="31">
+        <v>1269</v>
+      </c>
+      <c r="C612" s="31">
+        <v>2</v>
+      </c>
+      <c r="D612" s="31">
+        <v>101</v>
+      </c>
+      <c r="E612" s="34" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="613" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A613" s="32" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B613" s="33">
+        <v>538</v>
+      </c>
+      <c r="C613" s="33">
+        <v>7</v>
+      </c>
+      <c r="D613" s="33">
+        <v>65</v>
+      </c>
+      <c r="E613" s="35" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="614" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A614" s="32" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B614" s="33">
+        <v>487</v>
+      </c>
+      <c r="C614" s="33">
+        <v>0</v>
+      </c>
+      <c r="D614" s="33">
+        <v>33</v>
+      </c>
+      <c r="E614" s="35" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="615" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A615" s="32" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B615" s="33">
+        <v>756</v>
+      </c>
+      <c r="C615" s="33">
+        <v>13</v>
+      </c>
+      <c r="D615" s="33">
+        <v>39</v>
+      </c>
+      <c r="E615" s="35" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="616" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A616" s="32" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B616" s="33">
+        <v>809</v>
+      </c>
+      <c r="C616" s="33">
+        <v>1</v>
+      </c>
+      <c r="D616" s="33">
+        <v>68</v>
+      </c>
+      <c r="E616" s="35" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="617" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A617" s="32" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B617" s="33">
+        <v>1051</v>
+      </c>
+      <c r="C617" s="33">
+        <v>0</v>
+      </c>
+      <c r="D617" s="33">
+        <v>44</v>
+      </c>
+      <c r="E617" s="35" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="618" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A618" s="32" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B618" s="33">
+        <v>951</v>
+      </c>
+      <c r="C618" s="33">
+        <v>0</v>
+      </c>
+      <c r="D618" s="33">
+        <v>56</v>
+      </c>
+      <c r="E618" s="35" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A619" s="6" t="s">
         <v>483</v>
       </c>
@@ -14706,7 +14904,7 @@
       <c r="C619" s="5"/>
       <c r="D619" s="5"/>
     </row>
-    <row r="620" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A620" s="6" t="s">
         <v>483</v>
       </c>
@@ -14714,7 +14912,7 @@
       <c r="C620" s="5"/>
       <c r="D620" s="5"/>
     </row>
-    <row r="621" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A621" s="6" t="s">
         <v>483</v>
       </c>
@@ -14722,7 +14920,7 @@
       <c r="C621" s="5"/>
       <c r="D621" s="5"/>
     </row>
-    <row r="622" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="622" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A622" s="6" t="s">
         <v>483</v>
       </c>
@@ -14730,7 +14928,7 @@
       <c r="C622" s="5"/>
       <c r="D622" s="5"/>
     </row>
-    <row r="623" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A623" s="6" t="s">
         <v>483</v>
       </c>
@@ -14738,7 +14936,7 @@
       <c r="C623" s="5"/>
       <c r="D623" s="5"/>
     </row>
-    <row r="624" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="624" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A624" s="6" t="s">
         <v>483</v>
       </c>

</xml_diff>

<commit_message>
update for Boss Pack #3
</commit_message>
<xml_diff>
--- a/src/util/ecfa-parser/Songlist.xlsx
+++ b/src/util/ecfa-parser/Songlist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\source\repos\ecfa-react\src\util\ecfa-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\GitHub\ecfa-react\src\util\ecfa-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7A4511-540C-4E4C-AEBB-CC2B4A30FB9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21740B50-25BC-4C54-A54D-792473FE0E09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{771CF380-43F9-4460-B83F-E292DCFEC940}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1247">
   <si>
     <t>Rapid Fire (SH 7)</t>
   </si>
@@ -3739,13 +3739,49 @@
   </si>
   <si>
     <t>Prime Time (SX 14)</t>
+  </si>
+  <si>
+    <t>Blust of Wind</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t>Kurenai no panselinos</t>
+  </si>
+  <si>
+    <t>Agen Wida</t>
+  </si>
+  <si>
+    <t>Kamah -scythe-</t>
+  </si>
+  <si>
+    <t>Chaos Terror Tech Mix</t>
+  </si>
+  <si>
+    <t>Blust of Wind (SX 9)</t>
+  </si>
+  <si>
+    <t>Mantis (SX 10)</t>
+  </si>
+  <si>
+    <t>Kurenai no panselinos (SX 11)</t>
+  </si>
+  <si>
+    <t>Agen Wida (SX 12)</t>
+  </si>
+  <si>
+    <t>Kamah (Scythe) (SX 13)</t>
+  </si>
+  <si>
+    <t>CHAOS Terror-Tech Mix (SX 14)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3808,8 +3844,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF9900"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3864,8 +3913,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000089"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -3948,11 +4003,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4055,6 +4125,21 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4376,10 +4461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E9F61-E79C-418F-A754-D98BF653F3B5}">
-  <dimension ref="A1:E630"/>
+  <dimension ref="A1:E632"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E608" sqref="E608"/>
+    <sheetView tabSelected="1" topLeftCell="A608" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E619" sqref="E619:E624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14897,52 +14982,106 @@
       </c>
     </row>
     <row r="619" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A619" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B619" s="5"/>
-      <c r="C619" s="5"/>
-      <c r="D619" s="5"/>
+      <c r="A619" s="36" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B619" s="37">
+        <v>486</v>
+      </c>
+      <c r="C619" s="37">
+        <v>0</v>
+      </c>
+      <c r="D619" s="37">
+        <v>101</v>
+      </c>
+      <c r="E619" s="40" t="s">
+        <v>1241</v>
+      </c>
     </row>
     <row r="620" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A620" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B620" s="5"/>
-      <c r="C620" s="5"/>
-      <c r="D620" s="5"/>
+      <c r="A620" s="36" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B620" s="37">
+        <v>488</v>
+      </c>
+      <c r="C620" s="37">
+        <v>9</v>
+      </c>
+      <c r="D620" s="37">
+        <v>161</v>
+      </c>
+      <c r="E620" s="40" t="s">
+        <v>1242</v>
+      </c>
     </row>
     <row r="621" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A621" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B621" s="5"/>
-      <c r="C621" s="5"/>
-      <c r="D621" s="5"/>
+      <c r="A621" s="36" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B621" s="37">
+        <v>669</v>
+      </c>
+      <c r="C621" s="37">
+        <v>0</v>
+      </c>
+      <c r="D621" s="37">
+        <v>64</v>
+      </c>
+      <c r="E621" s="40" t="s">
+        <v>1243</v>
+      </c>
     </row>
     <row r="622" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A622" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B622" s="5"/>
-      <c r="C622" s="5"/>
-      <c r="D622" s="5"/>
+      <c r="A622" s="36" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B622" s="37">
+        <v>616</v>
+      </c>
+      <c r="C622" s="37">
+        <v>2</v>
+      </c>
+      <c r="D622" s="37">
+        <v>30</v>
+      </c>
+      <c r="E622" s="40" t="s">
+        <v>1244</v>
+      </c>
     </row>
     <row r="623" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A623" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B623" s="5"/>
-      <c r="C623" s="5"/>
-      <c r="D623" s="5"/>
+      <c r="A623" s="36" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B623" s="37">
+        <v>819</v>
+      </c>
+      <c r="C623" s="37">
+        <v>2</v>
+      </c>
+      <c r="D623" s="37">
+        <v>154</v>
+      </c>
+      <c r="E623" s="40" t="s">
+        <v>1245</v>
+      </c>
     </row>
     <row r="624" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A624" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B624" s="5"/>
-      <c r="C624" s="5"/>
-      <c r="D624" s="5"/>
+      <c r="A624" s="36" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B624" s="37">
+        <v>810</v>
+      </c>
+      <c r="C624" s="37">
+        <v>4</v>
+      </c>
+      <c r="D624" s="37">
+        <v>45</v>
+      </c>
+      <c r="E624" s="40" t="s">
+        <v>1246</v>
+      </c>
     </row>
     <row r="625" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A625" s="6" t="s">
@@ -14991,6 +15130,18 @@
       <c r="B630" s="5"/>
       <c r="C630" s="5"/>
       <c r="D630" s="5"/>
+    </row>
+    <row r="631" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A631" s="38"/>
+      <c r="B631" s="39"/>
+      <c r="C631" s="39"/>
+      <c r="D631" s="39"/>
+    </row>
+    <row r="632" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A632" s="38"/>
+      <c r="B632" s="39"/>
+      <c r="C632" s="39"/>
+      <c r="D632" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>